<commit_message>
Add new priority column and ensure numeric format for scores in export
</commit_message>
<xml_diff>
--- a/data_base/DS_TRUNGTUYEN_DOT.xlsx
+++ b/data_base/DS_TRUNGTUYEN_DOT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\ke-khai-gio-day-app-master\data_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{614B3928-28DE-4900-9E3F-4DEAA1F41F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DA4E52-9CF6-4408-9C25-9656146A0A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
  môn Văn </t>
   </si>
   <si>
-    <t xml:space="preserve">Tổng điểm </t>
-  </si>
-  <si>
     <t>Nam</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>Trương Thị Hoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng điểm môn </t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -494,6 +494,39 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -506,6 +539,12 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -524,80 +563,35 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,7 +969,7 @@
   <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2079,13 +2073,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="41"/>
       <c r="H1" s="8"/>
       <c r="I1" s="1"/>
       <c r="K1" s="11"/>
@@ -2097,13 +2091,13 @@
       <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
@@ -2112,122 +2106,122 @@
       <c r="I2" s="1"/>
       <c r="K2" s="11"/>
       <c r="M2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" s="11"/>
       <c r="O2" s="13"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53">
+      <c r="A3" s="45">
         <v>2025</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="53"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
+      <c r="A6" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="47"/>
+      <c r="X6" s="47"/>
+      <c r="Y6" s="47"/>
+      <c r="Z6" s="47"/>
     </row>
     <row r="7" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="str">
+      <c r="A7" s="47" t="str">
         <f>"NĂM HỌC "&amp;A3&amp;" - "&amp;A3+1</f>
         <v>NĂM HỌC 2025 - 2026</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+      <c r="X7" s="47"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="47"/>
     </row>
     <row r="8" spans="1:27" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="str">
+      <c r="A8" s="50" t="str">
         <f>"(Kèm theo Quyết định số ……....... /QĐ - CĐĐL ngày …........ tháng …....... năm "&amp;A3&amp;" của Trường Cao đẳng Đắk Lắk)"</f>
         <v>(Kèm theo Quyết định số ……....... /QĐ - CĐĐL ngày …........ tháng …....... năm 2025 của Trường Cao đẳng Đắk Lắk)</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="37"/>
-      <c r="W8" s="37"/>
-      <c r="X8" s="37"/>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="37"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="50"/>
     </row>
     <row r="9" spans="1:27" s="9" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="55" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="40" t="s">
@@ -2239,7 +2233,7 @@
       <c r="F9" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="58" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="40" t="s">
@@ -2257,119 +2251,119 @@
       <c r="L9" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="43" t="s">
+      <c r="N9" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="P9" s="44" t="s">
+      <c r="O9" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="P9" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44" t="s">
+      <c r="Q9" s="57"/>
+      <c r="R9" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="S9" s="44" t="s">
+      <c r="S9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="44" t="s">
+      <c r="T9" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="U9" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="V9" s="44" t="s">
+      <c r="U9" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="W9" s="45" t="s">
+      <c r="V9" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="W9" s="62" t="s">
         <v>19</v>
       </c>
       <c r="X9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="Y9" s="44" t="s">
+      <c r="Y9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="Z9" s="51" t="s">
+      <c r="Z9" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="AA9" s="52" t="s">
+      <c r="AA9" s="61" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:27" s="9" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
-      <c r="G10" s="48"/>
+      <c r="G10" s="59"/>
       <c r="H10" s="40"/>
       <c r="I10" s="40"/>
       <c r="J10" s="40"/>
       <c r="K10" s="40"/>
       <c r="L10" s="40"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="49" t="s">
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="Q10" s="50" t="s">
+      <c r="Q10" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="44"/>
-      <c r="U10" s="44"/>
-      <c r="V10" s="44"/>
-      <c r="W10" s="45"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="62"/>
       <c r="X10" s="40"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="51"/>
-      <c r="AA10" s="52"/>
+      <c r="Y10" s="57"/>
+      <c r="Z10" s="60"/>
+      <c r="AA10" s="61"/>
     </row>
     <row r="11" spans="1:27" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="D11" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="E11" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="J11" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="25" t="s">
         <v>35</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="L11" s="25" t="s">
-        <v>36</v>
       </c>
       <c r="M11" s="6">
         <v>6</v>
@@ -2395,57 +2389,73 @@
         <v>13.65</v>
       </c>
       <c r="U11" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V11" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W11" s="28">
         <v>2020</v>
       </c>
       <c r="X11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Z11" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="55"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="60"/>
-      <c r="S12" s="60"/>
-      <c r="T12" s="60"/>
-      <c r="U12" s="61"/>
-      <c r="V12" s="61"/>
-      <c r="W12" s="62"/>
-      <c r="X12" s="63"/>
-      <c r="Y12" s="64"/>
-      <c r="Z12" s="64"/>
-      <c r="AA12" s="64"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="38"/>
+      <c r="V12" s="38"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
     </row>
     <row r="13" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -2462,22 +2472,6 @@
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="Y9:Y10"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new data analysis page for student admission data
</commit_message>
<xml_diff>
--- a/data_base/DS_TRUNGTUYEN_DOT.xlsx
+++ b/data_base/DS_TRUNGTUYEN_DOT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\ke-khai-gio-day-app-master\data_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DA4E52-9CF6-4408-9C25-9656146A0A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C143AF76-199D-44BC-9CF2-44A1FEEF7049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,8 +203,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0;\-0.0;;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -409,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -424,9 +425,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -485,9 +483,6 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,21 +507,33 @@
     <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,23 +582,20 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -966,37 +970,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AF52DE-39BA-43E3-89C4-4D1731042B24}">
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="8" customWidth="1"/>
     <col min="2" max="2" width="20.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" style="9" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.75" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="8" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.125" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.25" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.375" style="7" customWidth="1"/>
     <col min="12" max="12" width="16.625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="6.875" style="8" customWidth="1"/>
-    <col min="15" max="15" width="7" style="16" customWidth="1"/>
-    <col min="16" max="16" width="6.625" style="14" customWidth="1"/>
-    <col min="17" max="17" width="6.625" style="15" customWidth="1"/>
-    <col min="18" max="20" width="7.625" style="16" customWidth="1"/>
-    <col min="21" max="21" width="22.25" style="16" customWidth="1"/>
-    <col min="22" max="22" width="6.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.875" style="17" customWidth="1"/>
-    <col min="24" max="24" width="14.25" style="18" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.625" style="19" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="16.125" style="20" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="6.875" style="7" customWidth="1"/>
+    <col min="15" max="15" width="7" style="15" customWidth="1"/>
+    <col min="16" max="16" width="6.625" style="13" customWidth="1"/>
+    <col min="17" max="17" width="6.625" style="14" customWidth="1"/>
+    <col min="18" max="20" width="7.625" style="15" customWidth="1"/>
+    <col min="21" max="21" width="22.25" style="15" customWidth="1"/>
+    <col min="22" max="22" width="6.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.875" style="16" customWidth="1"/>
+    <col min="24" max="24" width="14.25" style="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.625" style="18" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="16.125" style="19" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="252" width="9" style="1"/>
     <col min="253" max="253" width="6.625" style="1" customWidth="1"/>
@@ -2073,155 +2077,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="41"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="43"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="1"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="12" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="13"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="8" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="1"/>
-      <c r="K2" s="11"/>
-      <c r="M2" s="12" t="s">
+      <c r="K2" s="10"/>
+      <c r="M2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="13"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
+      <c r="A3" s="47">
         <v>2025</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="45"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
-      <c r="U6" s="47"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="47"/>
-      <c r="X6" s="47"/>
-      <c r="Y6" s="47"/>
-      <c r="Z6" s="47"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="49"/>
     </row>
     <row r="7" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="str">
+      <c r="A7" s="49" t="str">
         <f>"NĂM HỌC "&amp;A3&amp;" - "&amp;A3+1</f>
         <v>NĂM HỌC 2025 - 2026</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
-      <c r="T7" s="47"/>
-      <c r="U7" s="47"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="47"/>
-      <c r="X7" s="47"/>
-      <c r="Y7" s="47"/>
-      <c r="Z7" s="47"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="49"/>
     </row>
     <row r="8" spans="1:27" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="str">
+      <c r="A8" s="52" t="str">
         <f>"(Kèm theo Quyết định số ……....... /QĐ - CĐĐL ngày …........ tháng …....... năm "&amp;A3&amp;" của Trường Cao đẳng Đắk Lắk)"</f>
         <v>(Kèm theo Quyết định số ……....... /QĐ - CĐĐL ngày …........ tháng …....... năm 2025 của Trường Cao đẳng Đắk Lắk)</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="50"/>
-      <c r="V8" s="50"/>
-      <c r="W8" s="50"/>
-      <c r="X8" s="50"/>
-      <c r="Y8" s="50"/>
-      <c r="Z8" s="50"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="52"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="52"/>
+      <c r="X8" s="52"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="52"/>
     </row>
-    <row r="9" spans="1:27" s="9" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" s="8" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="57" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="40" t="s">
@@ -2233,7 +2237,7 @@
       <c r="F9" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="41" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="40" t="s">
@@ -2251,150 +2255,150 @@
       <c r="L9" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="58" t="s">
+      <c r="M9" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="58" t="s">
+      <c r="N9" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="57" t="s">
+      <c r="O9" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="57" t="s">
+      <c r="P9" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57" t="s">
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="S9" s="57" t="s">
+      <c r="S9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="57" t="s">
+      <c r="T9" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="U9" s="57" t="s">
+      <c r="U9" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="V9" s="57" t="s">
+      <c r="V9" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="W9" s="62" t="s">
+      <c r="W9" s="39" t="s">
         <v>19</v>
       </c>
       <c r="X9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="Y9" s="57" t="s">
+      <c r="Y9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="Z9" s="60" t="s">
+      <c r="Z9" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="AA9" s="61" t="s">
+      <c r="AA9" s="38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:27" s="9" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="8" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="56"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="58"/>
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
-      <c r="G10" s="59"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="40"/>
       <c r="I10" s="40"/>
       <c r="J10" s="40"/>
       <c r="K10" s="40"/>
       <c r="L10" s="40"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="31" t="s">
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="Q10" s="30" t="s">
+      <c r="Q10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="62"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="39"/>
       <c r="X10" s="40"/>
-      <c r="Y10" s="57"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="61"/>
+      <c r="Y10" s="36"/>
+      <c r="Z10" s="37"/>
+      <c r="AA10" s="38"/>
     </row>
     <row r="11" spans="1:27" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="K11" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="L11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="59">
         <v>6</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="59">
         <v>6.9</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="59">
         <f>SUM(M11:N11)</f>
         <v>12.9</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27">
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="59">
         <v>0.75</v>
       </c>
-      <c r="S11" s="27">
+      <c r="S11" s="59">
         <f>P11+R11</f>
         <v>0.75</v>
       </c>
-      <c r="T11" s="27">
+      <c r="T11" s="59">
         <f>O11+S11</f>
         <v>13.65</v>
       </c>
-      <c r="U11" s="26" t="s">
+      <c r="U11" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="26" t="s">
+      <c r="V11" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="W11" s="28">
+      <c r="W11" s="26">
         <v>2020</v>
       </c>
       <c r="X11" s="4" t="s">
@@ -2409,53 +2413,136 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="37"/>
-      <c r="T12" s="37"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="17"/>
-      <c r="X12" s="39"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="35"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
     </row>
-    <row r="13" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="62"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="62"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M15" s="61"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="61"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="62"/>
+      <c r="T16" s="62"/>
+    </row>
+    <row r="17" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M17" s="61"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+    </row>
+    <row r="18" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+    </row>
+    <row r="19" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M19" s="61"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="62"/>
+    </row>
+    <row r="20" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="61"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
+    </row>
+    <row r="21" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M21" s="61"/>
+      <c r="N21" s="61"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="61"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="62"/>
+      <c r="T21" s="62"/>
+    </row>
+    <row r="22" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="61"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="62"/>
+      <c r="T22" s="62"/>
+    </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -2472,6 +2559,22 @@
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>

</xml_diff>